<commit_message>
commiiting verify tabledata prgm
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davis\IdeaProjects\seleniumcommands\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9216FB67-A2B3-4423-A18C-0EE5BF348026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A7B224-A0B7-4670-85E3-FDD2066AA07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="W3table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -40,13 +41,76 @@
   </si>
   <si>
     <t>selenium222@test.com</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Alfreds Futterkiste</t>
+  </si>
+  <si>
+    <t>Maria Anders</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Centro comercial Moctezuma</t>
+  </si>
+  <si>
+    <t>Francisco Chang</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Ernst Handel</t>
+  </si>
+  <si>
+    <t>Roland Mendel</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Island Trading</t>
+  </si>
+  <si>
+    <t>Helen Bennett</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Laughing Bacchus Winecellars</t>
+  </si>
+  <si>
+    <t>Yoshi Tannamuri</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Magazzini Alimentari Riuniti</t>
+  </si>
+  <si>
+    <t>Giovanni Rovelli</t>
+  </si>
+  <si>
+    <t>Italy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,21 +126,226 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E9EB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -84,9 +353,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -370,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -420,4 +734,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A4E7C2-C6CA-4346-8BC3-66A14521B7E5}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>